<commit_message>
[DONE] Nova info Merce
Actualitzats valors excels.
</commit_message>
<xml_diff>
--- a/public/20211004_SUGGEREIX_Taula_A8.xlsx
+++ b/public/20211004_SUGGEREIX_Taula_A8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ficra-my.sharepoint.com/personal/mfont_icra_cat/Documents/Documentos/SUGGEREIX_Taules_transformades/Taules_SAD_actuals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_AD4D2F04E46CFB4ACB3E2009C513D486683EDF12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2901C0E-5321-4721-9488-E36225498192}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_AD4D2F04E46CFB4ACB3E2009C513D486683EDF12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4BC9342-6C45-4F3E-97CD-E0E38BD472BD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="65">
   <si>
     <t>Taula A8. Monitoratge de la qualitat microbiològica</t>
   </si>
@@ -232,49 +232,49 @@
     <t>Dummy9</t>
   </si>
   <si>
+    <t xml:space="preserve">El SAD recomanarà fer una avaluació específica del risc microbiològic per ajustar els VP definits pel RD 1620/2007. </t>
+  </si>
+  <si>
+    <t>Espores Clostridium perfringens</t>
+  </si>
+  <si>
+    <t>Industrial: neteja interior, indústria alimentària</t>
+  </si>
+  <si>
+    <t>Dummy10</t>
+  </si>
+  <si>
+    <t>Ambiental: recàrrega d'aqüífers per percolació</t>
+  </si>
+  <si>
+    <t>Dummy11</t>
+  </si>
+  <si>
+    <t>Valors per defecte de reducció logarítmica si no es disposa d'una avaluació específica del risc microbiològic. El SAD recomanarà fer una avaluació específica del risc microbiològic.</t>
+  </si>
+  <si>
+    <t>Ambiental: recàrrega d'aqüífers per injecció directa</t>
+  </si>
+  <si>
+    <t>Dummy12</t>
+  </si>
+  <si>
+    <t>Ambiental: reg de boscos i silvicultura</t>
+  </si>
+  <si>
+    <t>Dummy13</t>
+  </si>
+  <si>
+    <t>Valors de reducció logarítmica assumint una exposició semblant a la de l'ús 8.</t>
+  </si>
+  <si>
+    <t>Ambiental: altres usos (manteniment aiguamolls, cabals mínims i similars)</t>
+  </si>
+  <si>
+    <t>Dummy14</t>
+  </si>
+  <si>
     <t>nd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El SAD recomanarà fer una avaluació específica del risc microbiològic per ajustar els VP definits pel RD 1620/2007. </t>
-  </si>
-  <si>
-    <t>Espores Clostridium perfringens</t>
-  </si>
-  <si>
-    <t>Industrial: neteja interior, indústria alimentària</t>
-  </si>
-  <si>
-    <t>Dummy10</t>
-  </si>
-  <si>
-    <t>Ambiental: recàrrega d'aqüífers per percolació</t>
-  </si>
-  <si>
-    <t>Dummy11</t>
-  </si>
-  <si>
-    <t>Valors per defecte de reducció logarítmica si no es disposa d'una avaluació específica del risc microbiològic. El SAD recomanarà fer una avaluació específica del risc microbiològic.</t>
-  </si>
-  <si>
-    <t>Ambiental: recàrrega d'aqüífers per injecció directa</t>
-  </si>
-  <si>
-    <t>Dummy12</t>
-  </si>
-  <si>
-    <t>Ambiental: reg de boscos i silvicultura</t>
-  </si>
-  <si>
-    <t>Dummy13</t>
-  </si>
-  <si>
-    <t>Valors de reducció logarítmica assumint una exposició semblant a la de l'ús 8.</t>
-  </si>
-  <si>
-    <t>Ambiental: altres usos (manteniment aiguamolls, cabals mínims i similars)</t>
-  </si>
-  <si>
-    <t>Dummy14</t>
   </si>
   <si>
     <t>El SAD no especificarà valors de reducció log, però advertirà que caldria assolir els valors de reducció log necessaris per a l’ús 15 (prepotable) si l’aigua s’utilitzés amb aquesta finalitat més avall.</t>
@@ -359,7 +359,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -376,11 +376,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -426,6 +435,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -710,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -1669,10 +1691,11 @@
       <c r="E29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>46</v>
+      <c r="F29" s="3">
+        <v>0.5</v>
       </c>
       <c r="G29" s="11">
+        <f>1-10^-F29</f>
         <v>0.683772233983162</v>
       </c>
       <c r="H29" s="3">
@@ -1685,7 +1708,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L29" s="3"/>
     </row>
@@ -1705,10 +1728,11 @@
       <c r="E30" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>46</v>
+      <c r="F30" s="3">
+        <v>1</v>
       </c>
       <c r="G30" s="11">
+        <f t="shared" ref="G30:G31" si="2">1-10^-F30</f>
         <v>0.9</v>
       </c>
       <c r="H30" s="3"/>
@@ -1721,44 +1745,45 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:12" s="20" customFormat="1">
+      <c r="A31" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="D31" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G31" s="12">
+      <c r="F31" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="19">
+        <f t="shared" si="2"/>
         <v>0.683772233983162</v>
       </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" s="5">
-        <v>2</v>
-      </c>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="17">
+        <v>2</v>
+      </c>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>16</v>
@@ -1769,10 +1794,11 @@
       <c r="E32" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>46</v>
+      <c r="F32" s="3">
+        <v>1</v>
       </c>
       <c r="G32" s="3">
+        <f>1-10^-F32</f>
         <v>0.9</v>
       </c>
       <c r="H32" s="3">
@@ -1785,16 +1811,16 @@
         <v>2</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L32" s="3"/>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>22</v>
@@ -1805,10 +1831,11 @@
       <c r="E33" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>46</v>
+      <c r="F33" s="3">
+        <v>1</v>
       </c>
       <c r="G33" s="3">
+        <f t="shared" ref="G33:G34" si="3">1-10^-F33</f>
         <v>0.9</v>
       </c>
       <c r="H33" s="3"/>
@@ -1821,44 +1848,45 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:12" s="20" customFormat="1">
+      <c r="A34" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G34" s="5">
+      <c r="F34" s="17">
+        <v>1</v>
+      </c>
+      <c r="G34" s="17">
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="5">
-        <v>2</v>
-      </c>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="17">
+        <v>2</v>
+      </c>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>16</v>
@@ -1873,7 +1901,7 @@
         <v>8.1</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" ref="G35:G43" si="2">1-10^-F35</f>
+        <f t="shared" ref="G35:G43" si="4">1-10^-F35</f>
         <v>0.99999999205671763</v>
       </c>
       <c r="H35" s="3" t="s">
@@ -1886,16 +1914,16 @@
         <v>2</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L35" s="3"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>22</v>
@@ -1910,7 +1938,7 @@
         <v>9.5</v>
       </c>
       <c r="G36" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.99999999968377229</v>
       </c>
       <c r="H36" s="3" t="s">
@@ -1927,16 +1955,16 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>28</v>
@@ -1945,7 +1973,7 @@
         <v>8</v>
       </c>
       <c r="G37" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.99999998999999995</v>
       </c>
       <c r="H37" s="5" t="s">
@@ -1962,10 +1990,10 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>16</v>
@@ -1980,7 +2008,7 @@
         <v>8.1</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.99999999205671763</v>
       </c>
       <c r="H38" s="3" t="s">
@@ -1999,10 +2027,10 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>22</v>
@@ -2017,7 +2045,7 @@
         <v>9.5</v>
       </c>
       <c r="G39" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.99999999968377229</v>
       </c>
       <c r="H39" s="3" t="s">
@@ -2034,16 +2062,16 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>28</v>
@@ -2052,7 +2080,7 @@
         <v>8</v>
       </c>
       <c r="G40" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.99999998999999995</v>
       </c>
       <c r="H40" s="5" t="s">
@@ -2069,10 +2097,10 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>16</v>
@@ -2087,7 +2115,7 @@
         <v>0.5</v>
       </c>
       <c r="G41" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.683772233983162</v>
       </c>
       <c r="H41" s="3">
@@ -2100,16 +2128,16 @@
         <v>2</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L41" s="3"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>22</v>
@@ -2124,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.9</v>
       </c>
       <c r="H42" s="3"/>
@@ -2139,16 +2167,16 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>28</v>
@@ -2157,7 +2185,7 @@
         <v>0.5</v>
       </c>
       <c r="G43" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.683772233983162</v>
       </c>
       <c r="H43" s="5"/>
@@ -2172,10 +2200,10 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>16</v>
@@ -2187,13 +2215,13 @@
         <v>18</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>20</v>
@@ -2208,10 +2236,10 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>22</v>
@@ -2223,13 +2251,13 @@
         <v>24</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>25</v>
@@ -2242,28 +2270,28 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>20</v>
@@ -2331,7 +2359,7 @@
         <v>9.5</v>
       </c>
       <c r="G48" s="13">
-        <f t="shared" ref="G48:G49" si="3">1-10^-F48</f>
+        <f t="shared" ref="G48:G49" si="5">1-10^-F48</f>
         <v>0.99999999968377229</v>
       </c>
       <c r="H48" s="3" t="s">
@@ -2357,7 +2385,7 @@
         <v>26</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>28</v>
@@ -2366,7 +2394,7 @@
         <v>8</v>
       </c>
       <c r="G49" s="16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.99999998999999995</v>
       </c>
       <c r="H49" s="5" t="s">
@@ -2519,6 +2547,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2527,20 +2561,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE21E60D-E1CC-4A69-8AA3-53988CC240AF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{852EB891-0D76-4939-9FA3-CF4A15FD2059}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB1F7163-78CD-426A-9224-347D439CEBB2}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB1F7163-78CD-426A-9224-347D439CEBB2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{852EB891-0D76-4939-9FA3-CF4A15FD2059}"/>
 </file>
</xml_diff>